<commit_message>
updated analysis pipeline to include varied sizes and combinations tasks
updated tuning and decoding pipelines for new tasks. created decoding per timebin analysis. analyzed AN, FG, GB datasets
</commit_message>
<xml_diff>
--- a/ExcelFiles/s2_good_trials_GraspObject_Varied_Size.xlsx
+++ b/ExcelFiles/s2_good_trials_GraspObject_Varied_Size.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macthurston\Documents\GitHub\project_grasp_object_interaction\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E92F8B-FE5C-4FBA-8B08-E76FCA61C42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6932B6-A8D3-48F0-B9F6-DE52EE93D005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-3135" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -38,6 +38,60 @@
   </si>
   <si>
     <t>pilot</t>
+  </si>
+  <si>
+    <t>15,19,22,27</t>
+  </si>
+  <si>
+    <t>5,12,19,25</t>
+  </si>
+  <si>
+    <t>18,23,27</t>
+  </si>
+  <si>
+    <t>6,12,15,16,20,22,27,28</t>
+  </si>
+  <si>
+    <t>16,23</t>
+  </si>
+  <si>
+    <t>9,14,21</t>
+  </si>
+  <si>
+    <t>7,11,23</t>
+  </si>
+  <si>
+    <t>10,13,16,20</t>
+  </si>
+  <si>
+    <t>1,3,9,10,11,12,22,26</t>
+  </si>
+  <si>
+    <t>4,5,11,14,18,19,25,26</t>
+  </si>
+  <si>
+    <t>6,11,14,16,18,22,26</t>
+  </si>
+  <si>
+    <t>2,7,9,10,11,18,22,23,24</t>
+  </si>
+  <si>
+    <t>9,10,11,12,22,23,28</t>
+  </si>
+  <si>
+    <t>15,23,24,25,26</t>
+  </si>
+  <si>
+    <t>3,4,5,9,12,13,14,19,22,23,24,25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,10,15,21,22,23,24</t>
+  </si>
+  <si>
+    <t>1,2,3,8,13,15,18,19,20,26,27,28</t>
+  </si>
+  <si>
+    <t>1,2,3,9,10,12,17,21,25,26</t>
   </si>
 </sst>
 </file>
@@ -356,21 +410,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -429,6 +483,242 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20250312</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>20250328</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20250402</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20250501</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>20250517</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20250519</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>20250520</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18">
+        <v>23</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>